<commit_message>
Lösung Netzplanübung 2 - Übung 2
</commit_message>
<xml_diff>
--- a/FISID_Übungen/Netzplan_Übung2.xlsx
+++ b/FISID_Übungen/Netzplan_Übung2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FISID_Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87302A9-ADA1-43D6-85C2-089D6FA0DF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5049538E-64D8-453C-9E03-C1F9BE7DF3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übung1" sheetId="1" r:id="rId1"/>
     <sheet name="Übung 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Übung 3" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -303,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -315,6 +316,43 @@
       <left style="hair">
         <color auto="1"/>
       </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="hair">
         <color auto="1"/>
       </right>
@@ -444,6 +482,15 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -453,11 +500,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -521,26 +607,36 @@
     <xf numFmtId="0" fontId="7" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -549,12 +645,280 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="54">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1182,16 +1546,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1286,46 +1650,46 @@
         <f>SUM(CH3:CU3)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="K3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
       <c r="N3" s="23"/>
       <c r="O3" s="24"/>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="36"/>
-      <c r="R3" s="36"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
       <c r="S3" s="23"/>
       <c r="T3" s="24"/>
-      <c r="U3" s="36" t="s">
+      <c r="U3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
       <c r="X3" s="23"/>
       <c r="Y3" s="24"/>
-      <c r="Z3" s="36" t="s">
+      <c r="Z3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="36"/>
-      <c r="AB3" s="36"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
       <c r="AC3" s="23"/>
       <c r="AD3" s="24"/>
-      <c r="AE3" s="36" t="s">
+      <c r="AE3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AF3" s="36"/>
-      <c r="AG3" s="36"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
       <c r="AH3" s="23"/>
       <c r="AI3" s="24"/>
-      <c r="AJ3" s="36" t="s">
+      <c r="AJ3" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="AK3" s="36"/>
-      <c r="AL3" s="36"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -1617,25 +1981,25 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="28"/>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
       <c r="S9" s="23"/>
       <c r="T9" s="24"/>
-      <c r="U9" s="36" t="s">
+      <c r="U9" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
       <c r="X9" s="23"/>
       <c r="Y9" s="24"/>
-      <c r="Z9" s="36" t="s">
+      <c r="Z9" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="AA9" s="36"/>
-      <c r="AB9" s="36"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="37"/>
       <c r="AC9" s="29"/>
       <c r="AD9" s="27"/>
     </row>
@@ -1821,27 +2185,27 @@
       <c r="M15" s="27"/>
       <c r="N15" s="34"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="36" t="s">
+      <c r="P15" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="36"/>
-      <c r="R15" s="36"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
       <c r="S15" s="23"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="36" t="s">
+      <c r="U15" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="V15" s="36"/>
-      <c r="W15" s="36"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
       <c r="X15" s="23"/>
       <c r="Y15" s="24"/>
-      <c r="Z15" s="36" t="s">
+      <c r="Z15" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="AA15" s="36"/>
-      <c r="AB15" s="36"/>
+      <c r="AA15" s="37"/>
+      <c r="AB15" s="37"/>
       <c r="AC15" s="23"/>
-      <c r="AD15" s="39"/>
+      <c r="AD15" s="43"/>
     </row>
     <row r="16" spans="1:38">
       <c r="P16" s="18">
@@ -1914,35 +2278,35 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="H23" s="37" t="s">
+      <c r="A23" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="H23" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
     </row>
     <row r="24" spans="1:28">
       <c r="A24" s="18" t="s">
@@ -1957,17 +2321,17 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
     </row>
     <row r="25" spans="1:28">
       <c r="A25" s="21" t="s">
@@ -1980,17 +2344,17 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
     </row>
     <row r="27" spans="1:28" ht="13.5">
       <c r="J27" s="9"/>
@@ -2074,11 +2438,11 @@
     </row>
     <row r="42" spans="1:11" ht="13.5">
       <c r="A42" s="8"/>
-      <c r="B42" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
@@ -2270,67 +2634,67 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2345,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A829DA-0167-4E5C-96B8-1D44C392304E}">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:AQ53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
@@ -2356,20 +2720,20 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:43">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2377,7 +2741,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:43">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2400,8 +2764,34 @@
         <f>SUM(CH2:CU2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="K2" s="15">
+        <v>0</v>
+      </c>
+      <c r="L2" s="16"/>
+      <c r="M2" s="17">
+        <f>K2+K4</f>
+        <v>2</v>
+      </c>
+      <c r="P2" s="15">
+        <f>M2</f>
+        <v>2</v>
+      </c>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="17">
+        <f>P2+P4</f>
+        <v>10</v>
+      </c>
+      <c r="Z2" s="15">
+        <f>MAX(W8,R2)</f>
+        <v>16</v>
+      </c>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="17">
+        <f>Z2+Z4</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="13.5" thickBot="1">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2424,8 +2814,38 @@
         <f>SUM(CH3:CU3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="K3" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="35"/>
+      <c r="W3" s="35"/>
+      <c r="X3" s="35"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="35"/>
+      <c r="AE3" s="35"/>
+      <c r="AF3" s="35"/>
+      <c r="AG3" s="35"/>
+      <c r="AH3" s="35"/>
+    </row>
+    <row r="4" spans="1:43" ht="13.5" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -2446,8 +2866,47 @@
         <f>SUM(CH4:CU4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="K4" s="18">
+        <f>VLOOKUP(K3,$A$2:$H$13,8)</f>
+        <v>2</v>
+      </c>
+      <c r="L4" s="19">
+        <f>M5-M2</f>
+        <v>0</v>
+      </c>
+      <c r="M4" s="20">
+        <f>MIN(P2,U8,P14)-M2</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="25"/>
+      <c r="P4" s="18">
+        <f>VLOOKUP(P3,$A$2:$H$13,8)</f>
+        <v>8</v>
+      </c>
+      <c r="Q4" s="19">
+        <f>R5-R2</f>
+        <v>11</v>
+      </c>
+      <c r="R4" s="20">
+        <f>Z2-R2</f>
+        <v>6</v>
+      </c>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="18">
+        <f>VLOOKUP(Z3,$A$2:$H$13,8)</f>
+        <v>8</v>
+      </c>
+      <c r="AA4" s="19">
+        <f>AB5-AB2</f>
+        <v>5</v>
+      </c>
+      <c r="AB4" s="20">
+        <f>AJ8-AB2</f>
+        <v>5</v>
+      </c>
+      <c r="AH4" s="26"/>
+    </row>
+    <row r="5" spans="1:43">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2472,8 +2931,38 @@
         <f>SUM(CH5:CU5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="K5" s="21">
+        <f>M5-K4</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="22">
+        <f>MIN(P5,P17,U11)</f>
+        <v>2</v>
+      </c>
+      <c r="N5" s="26"/>
+      <c r="P5" s="21">
+        <f>R5-P4</f>
+        <v>13</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="22">
+        <f>Z5</f>
+        <v>21</v>
+      </c>
+      <c r="X5" s="27"/>
+      <c r="Z5" s="21">
+        <f>AB5-Z4</f>
+        <v>21</v>
+      </c>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="22">
+        <f>AJ11</f>
+        <v>29</v>
+      </c>
+      <c r="AH5" s="27"/>
+    </row>
+    <row r="6" spans="1:43">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -2496,15 +2985,21 @@
         <f t="shared" ref="I6:I13" si="0">SUM(BR6:CE6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="M6" s="33"/>
+      <c r="N6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="AH6" s="27"/>
+    </row>
+    <row r="7" spans="1:43">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="5" t="s">
         <v>4</v>
@@ -2518,8 +3013,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="X7" s="27"/>
+      <c r="AH7" s="27"/>
+    </row>
+    <row r="8" spans="1:43" ht="13.5" thickBot="1">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -2544,8 +3043,61 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="44"/>
+      <c r="U8" s="15">
+        <f>MAX(M2,R14)</f>
+        <v>10</v>
+      </c>
+      <c r="V8" s="16"/>
+      <c r="W8" s="17">
+        <f>U8+U10</f>
+        <v>16</v>
+      </c>
+      <c r="X8" s="29"/>
+      <c r="Z8" s="15">
+        <f>W8</f>
+        <v>16</v>
+      </c>
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="17">
+        <f>Z8+Z10</f>
+        <v>21</v>
+      </c>
+      <c r="AE8" s="15">
+        <f>MAX(AB8,W14)</f>
+        <v>21</v>
+      </c>
+      <c r="AF8" s="16"/>
+      <c r="AG8" s="17">
+        <f>AE8+AE10</f>
+        <v>29</v>
+      </c>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="28"/>
+      <c r="AJ8" s="15">
+        <f>MAX(AB2,AG8)</f>
+        <v>29</v>
+      </c>
+      <c r="AK8" s="16"/>
+      <c r="AL8" s="17">
+        <f>AJ8+AJ10</f>
+        <v>31</v>
+      </c>
+      <c r="AO8" s="15">
+        <f>MAX(AL8,AG14)</f>
+        <v>31</v>
+      </c>
+      <c r="AP8" s="16"/>
+      <c r="AQ8" s="17">
+        <f>AO8+AO10</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43" ht="13.5" thickBot="1">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -2566,8 +3118,49 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="M9" s="27"/>
+      <c r="N9" s="27"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="39"/>
+      <c r="AB9" s="40"/>
+      <c r="AC9" s="23"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF9" s="39"/>
+      <c r="AG9" s="40"/>
+      <c r="AH9" s="23"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK9" s="39"/>
+      <c r="AL9" s="40"/>
+      <c r="AM9" s="23"/>
+      <c r="AN9" s="24"/>
+      <c r="AO9" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="AP9" s="39"/>
+      <c r="AQ9" s="40"/>
+    </row>
+    <row r="10" spans="1:43" ht="13.5" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2588,8 +3181,72 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="M10" s="27"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="46"/>
+      <c r="T10" s="30"/>
+      <c r="U10" s="18">
+        <f>VLOOKUP(U9,$A$2:$H$13,8)</f>
+        <v>6</v>
+      </c>
+      <c r="V10" s="19">
+        <f>W11-W8</f>
+        <v>0</v>
+      </c>
+      <c r="W10" s="20">
+        <f>MIN(Z2,Z8)-W8</f>
+        <v>0</v>
+      </c>
+      <c r="Z10" s="18">
+        <f>VLOOKUP(Z9,$A$2:$H$13,8)</f>
+        <v>5</v>
+      </c>
+      <c r="AA10" s="19">
+        <f>AB11-AB8</f>
+        <v>0</v>
+      </c>
+      <c r="AB10" s="20">
+        <f>AE8-AB8</f>
+        <v>0</v>
+      </c>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="18">
+        <f>VLOOKUP(AE9,$A$2:$H$13,8)</f>
+        <v>8</v>
+      </c>
+      <c r="AF10" s="19">
+        <f>AG11-AG8</f>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="20">
+        <f>AJ8-AG8</f>
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="18">
+        <f>VLOOKUP(AJ9,$A$2:$H$13,8)</f>
+        <v>2</v>
+      </c>
+      <c r="AK10" s="19">
+        <f>AL11-AL8</f>
+        <v>0</v>
+      </c>
+      <c r="AL10" s="20">
+        <f>AO8-AL8</f>
+        <v>0</v>
+      </c>
+      <c r="AN10" s="30"/>
+      <c r="AO10" s="18">
+        <f>VLOOKUP(AO9,$A$2:$H$13,8)</f>
+        <v>4</v>
+      </c>
+      <c r="AP10" s="19">
+        <f>AQ11-AQ8</f>
+        <v>0</v>
+      </c>
+      <c r="AQ10" s="20"/>
+    </row>
+    <row r="11" spans="1:43">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -2612,8 +3269,60 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="M11" s="27"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="44"/>
+      <c r="S11" s="27"/>
+      <c r="U11" s="21">
+        <f>W11-U10</f>
+        <v>10</v>
+      </c>
+      <c r="V11" s="16"/>
+      <c r="W11" s="22">
+        <f>MIN(Z5,Z11)</f>
+        <v>16</v>
+      </c>
+      <c r="Z11" s="21">
+        <f>AB11-Z10</f>
+        <v>16</v>
+      </c>
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="22">
+        <f>AE11</f>
+        <v>21</v>
+      </c>
+      <c r="AC11" s="27"/>
+      <c r="AE11" s="21">
+        <f>AG11-AE10</f>
+        <v>21</v>
+      </c>
+      <c r="AF11" s="16"/>
+      <c r="AG11" s="22">
+        <f>AJ11</f>
+        <v>29</v>
+      </c>
+      <c r="AJ11" s="21">
+        <f>AL11-AJ10</f>
+        <v>29</v>
+      </c>
+      <c r="AK11" s="16"/>
+      <c r="AL11" s="22">
+        <f>AO11</f>
+        <v>31</v>
+      </c>
+      <c r="AM11" s="27"/>
+      <c r="AO11" s="21">
+        <f>AQ11-AO10</f>
+        <v>31</v>
+      </c>
+      <c r="AP11" s="16"/>
+      <c r="AQ11" s="22">
+        <f>AQ8</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43" ht="13.5" thickBot="1">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -2636,8 +3345,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="M12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="Y12" s="35"/>
+      <c r="Z12" s="35"/>
+      <c r="AA12" s="35"/>
+      <c r="AB12" s="35"/>
+      <c r="AC12" s="43"/>
+      <c r="AM12" s="27"/>
+    </row>
+    <row r="13" spans="1:43">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -2658,8 +3375,178 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="56.25">
+      <c r="M13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="X13" s="27"/>
+      <c r="AM13" s="27"/>
+    </row>
+    <row r="14" spans="1:43" ht="13.5" thickBot="1">
+      <c r="M14" s="27"/>
+      <c r="P14" s="15">
+        <f>M2</f>
+        <v>2</v>
+      </c>
+      <c r="Q14" s="16"/>
+      <c r="R14" s="17">
+        <f>P14+P16</f>
+        <v>10</v>
+      </c>
+      <c r="S14" s="49"/>
+      <c r="U14" s="15">
+        <f>R14</f>
+        <v>10</v>
+      </c>
+      <c r="V14" s="16"/>
+      <c r="W14" s="17">
+        <f>U14+U16</f>
+        <v>18</v>
+      </c>
+      <c r="X14" s="29"/>
+      <c r="Z14" s="15">
+        <f>W14</f>
+        <v>18</v>
+      </c>
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="17">
+        <f>Z14+Z16</f>
+        <v>24</v>
+      </c>
+      <c r="AE14" s="15">
+        <f>AB14</f>
+        <v>24</v>
+      </c>
+      <c r="AF14" s="16"/>
+      <c r="AG14" s="17">
+        <f>AE14+AE16</f>
+        <v>29</v>
+      </c>
+      <c r="AM14" s="27"/>
+    </row>
+    <row r="15" spans="1:43" ht="13.5" thickBot="1">
+      <c r="N15" s="34"/>
+      <c r="O15" s="24"/>
+      <c r="P15" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="29"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="40"/>
+      <c r="AC15" s="23"/>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF15" s="39"/>
+      <c r="AG15" s="40"/>
+      <c r="AH15" s="23"/>
+      <c r="AI15" s="35"/>
+      <c r="AJ15" s="35"/>
+      <c r="AK15" s="35"/>
+      <c r="AL15" s="35"/>
+      <c r="AM15" s="43"/>
+    </row>
+    <row r="16" spans="1:43">
+      <c r="P16" s="18">
+        <f>VLOOKUP(P15,$A$2:$H$13,8)</f>
+        <v>8</v>
+      </c>
+      <c r="Q16" s="19">
+        <f>R17-R14</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="20">
+        <f>MIN(U8,U14)-R14</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="18">
+        <f>VLOOKUP(U15,$A$2:$H$13,8)</f>
+        <v>8</v>
+      </c>
+      <c r="V16" s="19">
+        <f>W17-W14</f>
+        <v>2</v>
+      </c>
+      <c r="W16" s="20">
+        <f>MIN(Z14,AE8)-W14</f>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="18">
+        <f>VLOOKUP(Z15,$A$2:$H$13,8)</f>
+        <v>6</v>
+      </c>
+      <c r="AA16" s="19">
+        <f>AB17-AB14</f>
+        <v>2</v>
+      </c>
+      <c r="AB16" s="20">
+        <f>AE14-AB14</f>
+        <v>0</v>
+      </c>
+      <c r="AE16" s="18">
+        <f>VLOOKUP(AE15,$A$2:$H$13,8)</f>
+        <v>5</v>
+      </c>
+      <c r="AF16" s="19">
+        <f>AG17-AG14</f>
+        <v>2</v>
+      </c>
+      <c r="AG16" s="20">
+        <f>AO8-AG14</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:33">
+      <c r="P17" s="21">
+        <f>R17-P16</f>
+        <v>2</v>
+      </c>
+      <c r="Q17" s="16"/>
+      <c r="R17" s="22">
+        <f>MIN(U11,U17)</f>
+        <v>10</v>
+      </c>
+      <c r="U17" s="21">
+        <f>W17-U16</f>
+        <v>12</v>
+      </c>
+      <c r="V17" s="16"/>
+      <c r="W17" s="22">
+        <f>MIN(AE11,Z17)</f>
+        <v>20</v>
+      </c>
+      <c r="Z17" s="21">
+        <f>AB17-Z16</f>
+        <v>20</v>
+      </c>
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="22">
+        <f>AE17</f>
+        <v>26</v>
+      </c>
+      <c r="AE17" s="21">
+        <f>AG17-AE16</f>
+        <v>26</v>
+      </c>
+      <c r="AF17" s="16"/>
+      <c r="AG17" s="22">
+        <f>AO11</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" ht="56.25">
       <c r="A21" s="31" t="s">
         <v>30</v>
       </c>
@@ -2667,7 +3554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:33">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -2678,37 +3565,37 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-      <c r="L22" s="37"/>
-      <c r="M22" s="37"/>
-      <c r="N22" s="37"/>
-      <c r="O22" s="37"/>
-      <c r="P22" s="37"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="H23" s="37" t="s">
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="H23" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-      <c r="L23" s="37"/>
-      <c r="M23" s="37"/>
-      <c r="N23" s="37"/>
-      <c r="O23" s="37"/>
-      <c r="P23" s="37"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="1:33">
       <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
@@ -2721,19 +3608,19 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+    </row>
+    <row r="25" spans="1:33">
       <c r="A25" s="21" t="s">
         <v>21</v>
       </c>
@@ -2744,39 +3631,39 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="37" t="s">
+      <c r="H25" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-      <c r="L25" s="37"/>
-      <c r="M25" s="37"/>
-      <c r="N25" s="37"/>
-      <c r="O25" s="37"/>
-      <c r="P25" s="37"/>
-    </row>
-    <row r="27" spans="1:16" ht="13.5">
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+    </row>
+    <row r="27" spans="1:33" ht="13.5">
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:16" ht="13.5">
+    <row r="28" spans="1:33" ht="13.5">
       <c r="J28" s="10"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:16" ht="13.5">
+    <row r="29" spans="1:33" ht="13.5">
       <c r="J29" s="11"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:16" ht="13.5">
+    <row r="30" spans="1:33" ht="13.5">
       <c r="J30" s="10"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:16" ht="13.5">
+    <row r="31" spans="1:33" ht="13.5">
       <c r="J31" s="10"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:16" ht="13.5">
+    <row r="32" spans="1:33" ht="13.5">
       <c r="J32" s="10"/>
       <c r="K32" s="9"/>
     </row>
@@ -2838,11 +3725,779 @@
     </row>
     <row r="42" spans="1:11" ht="13.5">
       <c r="A42" s="8"/>
-      <c r="B42" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
+      <c r="B42" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+    </row>
+    <row r="43" spans="1:11" ht="13.5">
+      <c r="A43" s="8"/>
+      <c r="B43" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:11" ht="13.5">
+      <c r="A44" s="8"/>
+      <c r="B44" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" spans="1:11" ht="13.5">
+      <c r="A45" s="8"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:11" ht="13.5">
+      <c r="A46" s="8"/>
+      <c r="B46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:11" ht="13.5">
+      <c r="A47" s="8"/>
+      <c r="B47" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" ht="13.5">
+      <c r="A48" s="8"/>
+      <c r="B48" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+    </row>
+    <row r="49" spans="1:9" ht="13.5">
+      <c r="A49" s="8"/>
+      <c r="B49" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+    </row>
+    <row r="50" spans="1:9" ht="13.5">
+      <c r="A50" s="8"/>
+      <c r="B50" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" spans="1:9" ht="13.5">
+      <c r="A51" s="8"/>
+      <c r="B51" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" ht="13.5">
+      <c r="A52" s="8"/>
+      <c r="B52" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+    </row>
+    <row r="53" spans="1:9" ht="13.5">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="AJ9:AL9"/>
+    <mergeCell ref="AO9:AQ9"/>
+    <mergeCell ref="Z3:AB3"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="Z9:AB9"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="Z15:AB15"/>
+    <mergeCell ref="AE15:AG15"/>
+    <mergeCell ref="H25:P25"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H22:P22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="H23:P23"/>
+    <mergeCell ref="H24:P24"/>
+  </mergeCells>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q10">
+    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP10">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK10">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF10">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF16">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA10">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA4">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA16">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V16">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V10">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q16">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B27E56-D803-4C26-BC0D-EC09884D6C55}">
+  <dimension ref="A1:P53"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3">
+        <v>3</v>
+      </c>
+      <c r="I2" s="6">
+        <f>SUM(CH2:CU2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3">
+        <v>5</v>
+      </c>
+      <c r="I3" s="6">
+        <f>SUM(CH3:CU3)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3">
+        <v>7</v>
+      </c>
+      <c r="I4" s="6">
+        <f>SUM(CH4:CU4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3">
+        <v>9</v>
+      </c>
+      <c r="I5" s="6">
+        <f>SUM(CH5:CU5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="6">
+        <f t="shared" ref="I6:I13" si="0">SUM(BR6:CE6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3">
+        <v>11</v>
+      </c>
+      <c r="I7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+      <c r="I10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3">
+        <v>3</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3">
+        <v>8</v>
+      </c>
+      <c r="I13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="56.25">
+      <c r="A21" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="41"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="H23" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+      <c r="L23" s="41"/>
+      <c r="M23" s="41"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
+      <c r="P23" s="41"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+      <c r="K24" s="41"/>
+      <c r="L24" s="41"/>
+      <c r="M24" s="41"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
+      <c r="P24" s="41"/>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="16"/>
+      <c r="C25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25" s="41"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="P25" s="41"/>
+    </row>
+    <row r="27" spans="1:16" ht="13.5">
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:16" ht="13.5">
+      <c r="J28" s="10"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:16" ht="13.5">
+      <c r="J29" s="11"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="1:16" ht="13.5">
+      <c r="J30" s="10"/>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="1:16" ht="13.5">
+      <c r="J31" s="10"/>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:16" ht="13.5">
+      <c r="J32" s="10"/>
+      <c r="K32" s="9"/>
+    </row>
+    <row r="33" spans="1:11" ht="13.5">
+      <c r="J33" s="10"/>
+      <c r="K33" s="9"/>
+    </row>
+    <row r="34" spans="1:11" ht="13.5">
+      <c r="J34" s="10"/>
+      <c r="K34" s="9"/>
+    </row>
+    <row r="35" spans="1:11" ht="13.5">
+      <c r="J35" s="10"/>
+      <c r="K35" s="9"/>
+    </row>
+    <row r="36" spans="1:11" ht="13.5">
+      <c r="J36" s="10"/>
+      <c r="K36" s="9"/>
+    </row>
+    <row r="37" spans="1:11" ht="13.5">
+      <c r="J37" s="10"/>
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" ht="13.5">
+      <c r="J38" s="10"/>
+      <c r="K38" s="9"/>
+    </row>
+    <row r="39" spans="1:11" ht="13.5">
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
+    </row>
+    <row r="40" spans="1:11" ht="13.5">
+      <c r="A40" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+    </row>
+    <row r="41" spans="1:11" ht="13.5">
+      <c r="A41" s="8"/>
+      <c r="B41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:11" ht="13.5">
+      <c r="A42" s="8"/>
+      <c r="B42" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="42"/>
+      <c r="D42" s="42"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
@@ -3022,7 +4677,7 @@
     <mergeCell ref="H24:P24"/>
   </mergeCells>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Lösung Netzplan Übung 2 -> Übung 3
</commit_message>
<xml_diff>
--- a/FISID_Übungen/Netzplan_Übung2.xlsx
+++ b/FISID_Übungen/Netzplan_Übung2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Captiva\git\QM_PM\FISID_Übungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5049538E-64D8-453C-9E03-C1F9BE7DF3E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3FCE657-06CD-40A7-8DED-6CC66E9A07D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übung1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="39">
   <si>
     <t>ID</t>
   </si>
@@ -304,7 +304,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -459,6 +459,17 @@
       <diagonal/>
     </border>
     <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -543,7 +554,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -624,6 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -645,28 +657,137 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFF0000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1546,16 +1667,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1650,46 +1771,46 @@
         <f>SUM(CH3:CU3)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="23"/>
       <c r="O3" s="24"/>
-      <c r="P3" s="37" t="s">
+      <c r="P3" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
       <c r="S3" s="23"/>
       <c r="T3" s="24"/>
-      <c r="U3" s="37" t="s">
+      <c r="U3" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
       <c r="X3" s="23"/>
       <c r="Y3" s="24"/>
-      <c r="Z3" s="37" t="s">
+      <c r="Z3" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
       <c r="AC3" s="23"/>
       <c r="AD3" s="24"/>
-      <c r="AE3" s="37" t="s">
+      <c r="AE3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
       <c r="AH3" s="23"/>
       <c r="AI3" s="24"/>
-      <c r="AJ3" s="37" t="s">
+      <c r="AJ3" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
+      <c r="AK3" s="38"/>
+      <c r="AL3" s="38"/>
     </row>
     <row r="4" spans="1:38" ht="13.5" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -1866,7 +1987,7 @@
         <f t="shared" ref="I6:I13" si="0">SUM(BR6:CE6)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="33"/>
+      <c r="M6" s="34"/>
       <c r="N6" s="27"/>
       <c r="S6" s="27"/>
       <c r="X6" s="27"/>
@@ -1981,25 +2102,25 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="28"/>
-      <c r="P9" s="37" t="s">
+      <c r="P9" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
+      <c r="Q9" s="38"/>
+      <c r="R9" s="38"/>
       <c r="S9" s="23"/>
       <c r="T9" s="24"/>
-      <c r="U9" s="37" t="s">
+      <c r="U9" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
       <c r="X9" s="23"/>
       <c r="Y9" s="24"/>
-      <c r="Z9" s="37" t="s">
+      <c r="Z9" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="AA9" s="37"/>
-      <c r="AB9" s="37"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="38"/>
       <c r="AC9" s="29"/>
       <c r="AD9" s="27"/>
     </row>
@@ -2183,29 +2304,29 @@
     </row>
     <row r="15" spans="1:38" ht="13.5" thickBot="1">
       <c r="M15" s="27"/>
-      <c r="N15" s="34"/>
+      <c r="N15" s="35"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="37" t="s">
+      <c r="P15" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
       <c r="S15" s="23"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="37" t="s">
+      <c r="U15" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
       <c r="X15" s="23"/>
       <c r="Y15" s="24"/>
-      <c r="Z15" s="37" t="s">
+      <c r="Z15" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="AA15" s="37"/>
-      <c r="AB15" s="37"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="38"/>
       <c r="AC15" s="23"/>
-      <c r="AD15" s="43"/>
+      <c r="AD15" s="44"/>
     </row>
     <row r="16" spans="1:38">
       <c r="P16" s="18">
@@ -2278,35 +2399,35 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
     </row>
     <row r="23" spans="1:28">
-      <c r="A23" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="H23" s="41" t="s">
+      <c r="A23" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="H23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
     </row>
     <row r="24" spans="1:28">
       <c r="A24" s="18" t="s">
@@ -2321,17 +2442,17 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
     </row>
     <row r="25" spans="1:28">
       <c r="A25" s="21" t="s">
@@ -2344,17 +2465,17 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="41" t="s">
+      <c r="H25" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
     </row>
     <row r="27" spans="1:28" ht="13.5">
       <c r="J27" s="9"/>
@@ -2438,11 +2559,11 @@
     </row>
     <row r="42" spans="1:11" ht="13.5">
       <c r="A42" s="8"/>
-      <c r="B42" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
@@ -2634,67 +2755,67 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="52" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="40" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="cellIs" dxfId="38" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V4">
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4">
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2711,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A829DA-0167-4E5C-96B8-1D44C392304E}">
   <dimension ref="A1:AQ53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
@@ -2724,16 +2845,16 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -2814,36 +2935,36 @@
         <f>SUM(CH3:CU3)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="37" t="s">
+      <c r="K3" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="23"/>
       <c r="O3" s="24"/>
-      <c r="P3" s="37" t="s">
+      <c r="P3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="38"/>
       <c r="S3" s="23"/>
       <c r="T3" s="24"/>
       <c r="U3" s="23"/>
-      <c r="V3" s="35"/>
-      <c r="W3" s="35"/>
-      <c r="X3" s="35"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
       <c r="Y3" s="24"/>
-      <c r="Z3" s="37" t="s">
+      <c r="Z3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
+      <c r="AA3" s="38"/>
+      <c r="AB3" s="38"/>
       <c r="AC3" s="23"/>
-      <c r="AD3" s="35"/>
-      <c r="AE3" s="35"/>
-      <c r="AF3" s="35"/>
-      <c r="AG3" s="35"/>
-      <c r="AH3" s="35"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="36"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="36"/>
     </row>
     <row r="4" spans="1:43" ht="13.5" thickBot="1">
       <c r="A4" s="3" t="s">
@@ -2985,7 +3106,7 @@
         <f t="shared" ref="I6:I13" si="0">SUM(BR6:CE6)</f>
         <v>0</v>
       </c>
-      <c r="M6" s="33"/>
+      <c r="M6" s="34"/>
       <c r="N6" s="27"/>
       <c r="X6" s="27"/>
       <c r="AH6" s="27"/>
@@ -3045,9 +3166,9 @@
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="44"/>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="45"/>
       <c r="U8" s="15">
         <f>MAX(M2,R14)</f>
         <v>10</v>
@@ -3121,44 +3242,44 @@
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="28"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="49"/>
       <c r="S9" s="23"/>
       <c r="T9" s="24"/>
-      <c r="U9" s="37" t="s">
+      <c r="U9" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
+      <c r="V9" s="38"/>
+      <c r="W9" s="38"/>
       <c r="X9" s="23"/>
       <c r="Y9" s="24"/>
-      <c r="Z9" s="38" t="s">
+      <c r="Z9" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="40"/>
+      <c r="AA9" s="40"/>
+      <c r="AB9" s="41"/>
       <c r="AC9" s="23"/>
       <c r="AD9" s="24"/>
-      <c r="AE9" s="38" t="s">
+      <c r="AE9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AF9" s="39"/>
-      <c r="AG9" s="40"/>
+      <c r="AF9" s="40"/>
+      <c r="AG9" s="41"/>
       <c r="AH9" s="23"/>
       <c r="AI9" s="24"/>
-      <c r="AJ9" s="38" t="s">
+      <c r="AJ9" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="AK9" s="39"/>
-      <c r="AL9" s="40"/>
+      <c r="AK9" s="40"/>
+      <c r="AL9" s="41"/>
       <c r="AM9" s="23"/>
       <c r="AN9" s="24"/>
-      <c r="AO9" s="38" t="s">
+      <c r="AO9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="AP9" s="39"/>
-      <c r="AQ9" s="40"/>
+      <c r="AP9" s="40"/>
+      <c r="AQ9" s="41"/>
     </row>
     <row r="10" spans="1:43" ht="13.5" thickBot="1">
       <c r="A10" s="3" t="s">
@@ -3182,9 +3303,9 @@
         <v>0</v>
       </c>
       <c r="M10" s="27"/>
-      <c r="P10" s="46"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="46"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="47"/>
       <c r="T10" s="30"/>
       <c r="U10" s="18">
         <f>VLOOKUP(U9,$A$2:$H$13,8)</f>
@@ -3270,9 +3391,9 @@
         <v>0</v>
       </c>
       <c r="M11" s="27"/>
-      <c r="P11" s="44"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="44"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="45"/>
       <c r="S11" s="27"/>
       <c r="U11" s="21">
         <f>W11-U10</f>
@@ -3347,11 +3468,11 @@
       </c>
       <c r="M12" s="27"/>
       <c r="S12" s="27"/>
-      <c r="Y12" s="35"/>
-      <c r="Z12" s="35"/>
-      <c r="AA12" s="35"/>
-      <c r="AB12" s="35"/>
-      <c r="AC12" s="43"/>
+      <c r="Y12" s="36"/>
+      <c r="Z12" s="36"/>
+      <c r="AA12" s="36"/>
+      <c r="AB12" s="36"/>
+      <c r="AC12" s="44"/>
       <c r="AM12" s="27"/>
     </row>
     <row r="13" spans="1:43">
@@ -3391,7 +3512,7 @@
         <f>P14+P16</f>
         <v>10</v>
       </c>
-      <c r="S14" s="49"/>
+      <c r="S14" s="50"/>
       <c r="U14" s="15">
         <f>R14</f>
         <v>10</v>
@@ -3423,40 +3544,40 @@
       <c r="AM14" s="27"/>
     </row>
     <row r="15" spans="1:43" ht="13.5" thickBot="1">
-      <c r="N15" s="34"/>
+      <c r="N15" s="35"/>
       <c r="O15" s="24"/>
-      <c r="P15" s="37" t="s">
+      <c r="P15" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
       <c r="S15" s="29"/>
       <c r="T15" s="24"/>
-      <c r="U15" s="37" t="s">
+      <c r="U15" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="38"/>
       <c r="X15" s="23"/>
       <c r="Y15" s="24"/>
-      <c r="Z15" s="38" t="s">
+      <c r="Z15" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="40"/>
+      <c r="AA15" s="40"/>
+      <c r="AB15" s="41"/>
       <c r="AC15" s="23"/>
       <c r="AD15" s="24"/>
-      <c r="AE15" s="38" t="s">
+      <c r="AE15" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AF15" s="39"/>
-      <c r="AG15" s="40"/>
+      <c r="AF15" s="40"/>
+      <c r="AG15" s="41"/>
       <c r="AH15" s="23"/>
-      <c r="AI15" s="35"/>
-      <c r="AJ15" s="35"/>
-      <c r="AK15" s="35"/>
-      <c r="AL15" s="35"/>
-      <c r="AM15" s="43"/>
+      <c r="AI15" s="36"/>
+      <c r="AJ15" s="36"/>
+      <c r="AK15" s="36"/>
+      <c r="AL15" s="36"/>
+      <c r="AM15" s="44"/>
     </row>
     <row r="16" spans="1:43">
       <c r="P16" s="18">
@@ -3565,35 +3686,35 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
     </row>
     <row r="23" spans="1:33">
-      <c r="A23" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="H23" s="41" t="s">
+      <c r="A23" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="H23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
     </row>
     <row r="24" spans="1:33">
       <c r="A24" s="18" t="s">
@@ -3608,17 +3729,17 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
     </row>
     <row r="25" spans="1:33">
       <c r="A25" s="21" t="s">
@@ -3631,17 +3752,17 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="41" t="s">
+      <c r="H25" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
     </row>
     <row r="27" spans="1:33" ht="13.5">
       <c r="J27" s="9"/>
@@ -3725,11 +3846,11 @@
     </row>
     <row r="42" spans="1:11" ht="13.5">
       <c r="A42" s="8"/>
-      <c r="B42" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
@@ -3922,72 +4043,72 @@
     <mergeCell ref="H24:P24"/>
   </mergeCells>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="28" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="27" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="cellIs" dxfId="25" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="24" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AP10">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK10">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF10">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF16">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA10">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA16">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V16">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V10">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q16">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4002,10 +4123,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9B27E56-D803-4C26-BC0D-EC09884D6C55}">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:AM53"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.85546875" defaultRowHeight="12.75"/>
@@ -4013,20 +4134,20 @@
     <col min="1" max="1" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:39">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
@@ -4034,7 +4155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:39">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -4056,7 +4177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:39">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -4079,8 +4200,61 @@
         <f>SUM(CH3:CU3)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="L3" s="15">
+        <v>0</v>
+      </c>
+      <c r="M3" s="16"/>
+      <c r="N3" s="17">
+        <f>L3+L5</f>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="15">
+        <f>N3</f>
+        <v>3</v>
+      </c>
+      <c r="R3" s="16"/>
+      <c r="S3" s="17">
+        <f>Q3+Q5</f>
+        <v>8</v>
+      </c>
+      <c r="V3" s="15">
+        <f>S3</f>
+        <v>8</v>
+      </c>
+      <c r="W3" s="16"/>
+      <c r="X3" s="17">
+        <f>V3+V5</f>
+        <v>15</v>
+      </c>
+      <c r="AA3" s="15">
+        <f>X3</f>
+        <v>15</v>
+      </c>
+      <c r="AB3" s="16"/>
+      <c r="AC3" s="17">
+        <f>AA3+AA5</f>
+        <v>19</v>
+      </c>
+      <c r="AF3" s="15">
+        <f>AC3</f>
+        <v>19</v>
+      </c>
+      <c r="AG3" s="16"/>
+      <c r="AH3" s="17">
+        <f>AF3+AF5</f>
+        <v>25</v>
+      </c>
+      <c r="AK3" s="15">
+        <f>MAX(AH3,AH9,AH22)</f>
+        <v>31</v>
+      </c>
+      <c r="AL3" s="16"/>
+      <c r="AM3" s="17">
+        <f>AK3+AK5</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" ht="13.5" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -4103,8 +4277,48 @@
         <f>SUM(CH4:CU4)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="L4" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="23"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="23"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="23"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+    </row>
+    <row r="5" spans="1:39" ht="13.5" thickBot="1">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -4129,8 +4343,83 @@
         <f>SUM(CH5:CU5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="L5" s="18">
+        <f>VLOOKUP(L4,$A$2:$H$13,8)</f>
+        <v>3</v>
+      </c>
+      <c r="M5" s="19">
+        <f>N6-N3</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="20">
+        <f>MIN(Q3,V15)-N3</f>
+        <v>0</v>
+      </c>
+      <c r="O5" s="25"/>
+      <c r="Q5" s="18">
+        <f>VLOOKUP(Q4,$A$2:$H$13,8)</f>
+        <v>5</v>
+      </c>
+      <c r="R5" s="19">
+        <f>S6-S3</f>
+        <v>0</v>
+      </c>
+      <c r="S5" s="20">
+        <f>MIN(V3,V15)-S3</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="23"/>
+      <c r="V5" s="18">
+        <f>VLOOKUP(V4,$A$2:$H$13,8)</f>
+        <v>7</v>
+      </c>
+      <c r="W5" s="19">
+        <f>X6-X3</f>
+        <v>6</v>
+      </c>
+      <c r="X5" s="20">
+        <f>MIN(AA3,AA9)-X3</f>
+        <v>0</v>
+      </c>
+      <c r="Y5" s="25"/>
+      <c r="AA5" s="18">
+        <f>VLOOKUP(AA4,$A$2:$H$13,8)</f>
+        <v>4</v>
+      </c>
+      <c r="AB5" s="19">
+        <f>AC6-AC3</f>
+        <v>6</v>
+      </c>
+      <c r="AC5" s="20">
+        <f>AF3-AC3</f>
+        <v>0</v>
+      </c>
+      <c r="AF5" s="18">
+        <f>VLOOKUP(AF4,$A$2:$H$13,8)</f>
+        <v>6</v>
+      </c>
+      <c r="AG5" s="19">
+        <f>AH6-AH3</f>
+        <v>6</v>
+      </c>
+      <c r="AH5" s="20">
+        <f>$AK$3-AH3</f>
+        <v>6</v>
+      </c>
+      <c r="AJ5" s="30"/>
+      <c r="AK5" s="18">
+        <f>VLOOKUP(AK4,$A$2:$H$13,8)</f>
+        <v>2</v>
+      </c>
+      <c r="AL5" s="19">
+        <f>AM6-AM3</f>
+        <v>0</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -4151,8 +4440,66 @@
         <f t="shared" ref="I6:I13" si="0">SUM(BR6:CE6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="L6" s="21">
+        <f>N6-L5</f>
+        <v>0</v>
+      </c>
+      <c r="M6" s="16"/>
+      <c r="N6" s="22">
+        <f>MIN(Q6,V18)</f>
+        <v>3</v>
+      </c>
+      <c r="O6" s="26"/>
+      <c r="Q6" s="21">
+        <f>S6-Q5</f>
+        <v>3</v>
+      </c>
+      <c r="R6" s="16"/>
+      <c r="S6" s="22">
+        <f>MIN(V6,V18)</f>
+        <v>8</v>
+      </c>
+      <c r="T6" s="26"/>
+      <c r="V6" s="21">
+        <f>X6-V5</f>
+        <v>14</v>
+      </c>
+      <c r="W6" s="16"/>
+      <c r="X6" s="22">
+        <f>MIN(AA6,AA12)</f>
+        <v>21</v>
+      </c>
+      <c r="Y6" s="26"/>
+      <c r="AA6" s="21">
+        <f>AC6-AA5</f>
+        <v>21</v>
+      </c>
+      <c r="AB6" s="16"/>
+      <c r="AC6" s="22">
+        <f>AF6</f>
+        <v>25</v>
+      </c>
+      <c r="AF6" s="21">
+        <f>AH6-AF5</f>
+        <v>25</v>
+      </c>
+      <c r="AG6" s="16"/>
+      <c r="AH6" s="22">
+        <f>$AK$6</f>
+        <v>31</v>
+      </c>
+      <c r="AI6" s="27"/>
+      <c r="AK6" s="21">
+        <f>AM6-AK5</f>
+        <v>31</v>
+      </c>
+      <c r="AL6" s="16"/>
+      <c r="AM6" s="22">
+        <f>AM3</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39">
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
@@ -4173,8 +4520,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="O7" s="27"/>
+      <c r="T7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="AI7" s="27"/>
+      <c r="AJ7" s="27"/>
+    </row>
+    <row r="8" spans="1:39">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -4199,8 +4551,13 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="O8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+    </row>
+    <row r="9" spans="1:39">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
@@ -4221,8 +4578,36 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="O9" s="27"/>
+      <c r="P9" s="51"/>
+      <c r="Q9" s="51"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="27"/>
+      <c r="U9" s="51"/>
+      <c r="Y9" s="27"/>
+      <c r="AA9" s="15">
+        <f>X3</f>
+        <v>15</v>
+      </c>
+      <c r="AB9" s="16"/>
+      <c r="AC9" s="17">
+        <f>AA9+AA11</f>
+        <v>18</v>
+      </c>
+      <c r="AF9" s="15">
+        <f>MAX(AC9,AC15)</f>
+        <v>28</v>
+      </c>
+      <c r="AG9" s="16"/>
+      <c r="AH9" s="17">
+        <f>AF9+AF11</f>
+        <v>31</v>
+      </c>
+      <c r="AI9" s="27"/>
+      <c r="AJ9" s="27"/>
+    </row>
+    <row r="10" spans="1:39" ht="13.5" thickBot="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -4243,8 +4628,31 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="O10" s="27"/>
+      <c r="P10" s="51"/>
+      <c r="Q10" s="51"/>
+      <c r="R10" s="51"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="27"/>
+      <c r="U10" s="51"/>
+      <c r="Y10" s="27"/>
+      <c r="Z10" s="28"/>
+      <c r="AA10" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="23"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG10" s="38"/>
+      <c r="AH10" s="38"/>
+      <c r="AI10" s="29"/>
+      <c r="AJ10" s="27"/>
+    </row>
+    <row r="11" spans="1:39" ht="13.5" thickBot="1">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -4265,8 +4673,37 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="O11" s="27"/>
+      <c r="T11" s="27"/>
+      <c r="AA11" s="18">
+        <f>VLOOKUP(AA10,$A$2:$H$13,8)</f>
+        <v>3</v>
+      </c>
+      <c r="AB11" s="19">
+        <f>AC12-AC9</f>
+        <v>10</v>
+      </c>
+      <c r="AC11" s="20">
+        <f>AF9-AC9</f>
+        <v>10</v>
+      </c>
+      <c r="AD11" s="33"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="18">
+        <f>VLOOKUP(AF10,$A$2:$H$13,8)</f>
+        <v>3</v>
+      </c>
+      <c r="AG11" s="19">
+        <f>AH12-AH9</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" s="20">
+        <f>$AK$3-AH9</f>
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="27"/>
+    </row>
+    <row r="12" spans="1:39">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -4289,8 +4726,30 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="O12" s="27"/>
+      <c r="T12" s="27"/>
+      <c r="AA12" s="21">
+        <f>AC12-AA11</f>
+        <v>25</v>
+      </c>
+      <c r="AB12" s="16"/>
+      <c r="AC12" s="22">
+        <f>AF12</f>
+        <v>28</v>
+      </c>
+      <c r="AD12" s="27"/>
+      <c r="AF12" s="21">
+        <f>AH12-AF11</f>
+        <v>28</v>
+      </c>
+      <c r="AG12" s="16"/>
+      <c r="AH12" s="22">
+        <f>$AK$6</f>
+        <v>31</v>
+      </c>
+      <c r="AJ12" s="27"/>
+    </row>
+    <row r="13" spans="1:39">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -4313,16 +4772,134 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="56.25">
+      <c r="O13" s="27"/>
+      <c r="T13" s="27"/>
+      <c r="AD13" s="27"/>
+      <c r="AJ13" s="27"/>
+    </row>
+    <row r="14" spans="1:39">
+      <c r="O14" s="27"/>
+      <c r="T14" s="27"/>
+      <c r="AD14" s="27"/>
+      <c r="AJ14" s="27"/>
+    </row>
+    <row r="15" spans="1:39" ht="13.5" thickBot="1">
+      <c r="O15" s="27"/>
+      <c r="T15" s="27"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="15">
+        <f>MAX(N3,S3)</f>
+        <v>8</v>
+      </c>
+      <c r="W15" s="16"/>
+      <c r="X15" s="17">
+        <f>V15+V17</f>
+        <v>17</v>
+      </c>
+      <c r="AA15" s="15">
+        <f>X15</f>
+        <v>17</v>
+      </c>
+      <c r="AB15" s="16"/>
+      <c r="AC15" s="17">
+        <f>AA15+AA17</f>
+        <v>28</v>
+      </c>
+      <c r="AD15" s="27"/>
+      <c r="AJ15" s="27"/>
+    </row>
+    <row r="16" spans="1:39" ht="13.5" thickBot="1">
+      <c r="O16" s="27"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="36"/>
+      <c r="S16" s="36"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="24"/>
+      <c r="V16" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="W16" s="38"/>
+      <c r="X16" s="38"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB16" s="38"/>
+      <c r="AC16" s="38"/>
+      <c r="AD16" s="29"/>
+      <c r="AJ16" s="27"/>
+    </row>
+    <row r="17" spans="1:36" ht="13.5" thickBot="1">
+      <c r="V17" s="18">
+        <f>VLOOKUP(V16,$A$2:$H$13,8)</f>
+        <v>9</v>
+      </c>
+      <c r="W17" s="19">
+        <f>X18-X15</f>
+        <v>0</v>
+      </c>
+      <c r="X17" s="20">
+        <f>MIN(AA15,AA22)-X15</f>
+        <v>0</v>
+      </c>
+      <c r="Y17" s="25"/>
+      <c r="AA17" s="18">
+        <f>VLOOKUP(AA16,$A$2:$H$13,8)</f>
+        <v>11</v>
+      </c>
+      <c r="AB17" s="19">
+        <f>AC18-AC15</f>
+        <v>0</v>
+      </c>
+      <c r="AC17" s="20">
+        <f>AF9-AC15</f>
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="27"/>
+    </row>
+    <row r="18" spans="1:36">
+      <c r="V18" s="21">
+        <f>X18-V17</f>
+        <v>8</v>
+      </c>
+      <c r="W18" s="16"/>
+      <c r="X18" s="22">
+        <f>MIN(AA18,AA25)</f>
+        <v>17</v>
+      </c>
+      <c r="Y18" s="26"/>
+      <c r="AA18" s="21">
+        <f>AC18-AA17</f>
+        <v>17</v>
+      </c>
+      <c r="AB18" s="16"/>
+      <c r="AC18" s="22">
+        <f>AF12</f>
+        <v>28</v>
+      </c>
+      <c r="AJ18" s="27"/>
+    </row>
+    <row r="19" spans="1:36">
+      <c r="Y19" s="27"/>
+      <c r="AJ19" s="27"/>
+    </row>
+    <row r="20" spans="1:36">
+      <c r="Y20" s="27"/>
+      <c r="AJ20" s="27"/>
+    </row>
+    <row r="21" spans="1:36" ht="56.25">
       <c r="A21" s="31" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Y21" s="27"/>
+      <c r="AJ21" s="27"/>
+    </row>
+    <row r="22" spans="1:36">
       <c r="A22" s="15" t="s">
         <v>16</v>
       </c>
@@ -4333,37 +4910,73 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
-      <c r="H22" s="41" t="s">
+      <c r="H22" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="41"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="41"/>
-    </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="37"/>
-      <c r="H23" s="41" t="s">
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="42"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Y22" s="27"/>
+      <c r="AA22" s="15">
+        <f>X15</f>
+        <v>17</v>
+      </c>
+      <c r="AB22" s="16"/>
+      <c r="AC22" s="17">
+        <f>AA22+AA24</f>
+        <v>22</v>
+      </c>
+      <c r="AF22" s="15">
+        <f>AC22</f>
+        <v>22</v>
+      </c>
+      <c r="AG22" s="16"/>
+      <c r="AH22" s="17">
+        <f>AF22+AF24</f>
+        <v>24</v>
+      </c>
+      <c r="AJ22" s="27"/>
+    </row>
+    <row r="23" spans="1:36" ht="13.5" thickBot="1">
+      <c r="A23" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="H23" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="41"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
-      <c r="P23" s="41"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="42"/>
+      <c r="M23" s="42"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="42"/>
+      <c r="P23" s="42"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="23"/>
+      <c r="AE23" s="24"/>
+      <c r="AF23" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="38"/>
+      <c r="AI23" s="23"/>
+      <c r="AJ23" s="44"/>
+    </row>
+    <row r="24" spans="1:36">
       <c r="A24" s="18" t="s">
         <v>3</v>
       </c>
@@ -4376,19 +4989,43 @@
       <c r="D24" t="s">
         <v>33</v>
       </c>
-      <c r="H24" s="41" t="s">
+      <c r="H24" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="I24" s="41"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="P24" s="41"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="AA24" s="18">
+        <f>VLOOKUP(AA23,$A$2:$H$13,8)</f>
+        <v>5</v>
+      </c>
+      <c r="AB24" s="19">
+        <f>AC25-AC22</f>
+        <v>7</v>
+      </c>
+      <c r="AC24" s="20">
+        <f>AF22-AC22</f>
+        <v>0</v>
+      </c>
+      <c r="AF24" s="18">
+        <f>VLOOKUP(AF23,$A$2:$H$13,8)</f>
+        <v>2</v>
+      </c>
+      <c r="AG24" s="19">
+        <f>AH25-AH22</f>
+        <v>7</v>
+      </c>
+      <c r="AH24" s="20">
+        <f>$AK$3-AH22</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36">
       <c r="A25" s="21" t="s">
         <v>21</v>
       </c>
@@ -4399,39 +5036,57 @@
       <c r="D25" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="41" t="s">
+      <c r="H25" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="P25" s="41"/>
-    </row>
-    <row r="27" spans="1:16" ht="13.5">
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="AA25" s="21">
+        <f>AC25-AA24</f>
+        <v>24</v>
+      </c>
+      <c r="AB25" s="16"/>
+      <c r="AC25" s="22">
+        <f>AF25</f>
+        <v>29</v>
+      </c>
+      <c r="AF25" s="21">
+        <f>AH25-AF24</f>
+        <v>29</v>
+      </c>
+      <c r="AG25" s="16"/>
+      <c r="AH25" s="22">
+        <f>$AK$6</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:36" ht="13.5">
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:16" ht="13.5">
+    <row r="28" spans="1:36" ht="13.5">
       <c r="J28" s="10"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:16" ht="13.5">
+    <row r="29" spans="1:36" ht="13.5">
       <c r="J29" s="11"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:16" ht="13.5">
+    <row r="30" spans="1:36" ht="13.5">
       <c r="J30" s="10"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:16" ht="13.5">
+    <row r="31" spans="1:36" ht="13.5">
       <c r="J31" s="10"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:16" ht="13.5">
+    <row r="32" spans="1:36" ht="13.5">
       <c r="J32" s="10"/>
       <c r="K32" s="9"/>
     </row>
@@ -4493,11 +5148,11 @@
     </row>
     <row r="42" spans="1:11" ht="13.5">
       <c r="A42" s="8"/>
-      <c r="B42" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="C42" s="42"/>
-      <c r="D42" s="42"/>
+      <c r="B42" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
       <c r="E42" s="10"/>
       <c r="F42" s="11" t="s">
         <v>18</v>
@@ -4666,9 +5321,21 @@
       <c r="I53" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="20">
+    <mergeCell ref="AK4:AM4"/>
+    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="AA10:AC10"/>
+    <mergeCell ref="AA16:AC16"/>
+    <mergeCell ref="AA23:AC23"/>
+    <mergeCell ref="AF4:AH4"/>
+    <mergeCell ref="AF10:AH10"/>
+    <mergeCell ref="AF23:AH23"/>
     <mergeCell ref="H25:P25"/>
     <mergeCell ref="B42:D42"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="V4:X4"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H22:P22"/>
@@ -4677,7 +5344,67 @@
     <mergeCell ref="H24:P24"/>
   </mergeCells>
   <conditionalFormatting sqref="B24">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M5">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R5">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W17">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="W5">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB5">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB11">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB17">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB24">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG5">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG11">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG24">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL5">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>